<commit_message>
actualizacion cls cargue formularios
</commit_message>
<xml_diff>
--- a/data/upload_soul/Axa Falabella/PLACAS.xlsx
+++ b/data/upload_soul/Axa Falabella/PLACAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson.Aguilar\Documents\git_hub\Axa\data\upload_soul\Axa Falabella\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AA73D4-FD2E-4056-9371-A6D7FA3C3306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD90CBC-A157-4B0C-8FCA-608883A82FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95C444D8-FD0D-4D5B-800F-070C7EDD79D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{95C444D8-FD0D-4D5B-800F-070C7EDD79D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
     <t>SANTA MARTA</t>
   </si>
   <si>
-    <t>Cedula</t>
+    <t>CC</t>
   </si>
 </sst>
 </file>
@@ -329,28 +329,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -683,53 +662,53 @@
   <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="27" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -967,7 +946,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1086,7 +1065,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>

</xml_diff>